<commit_message>
Painted to cells in purple for testing purposes
</commit_message>
<xml_diff>
--- a/MOOCs tracker.xlsx
+++ b/MOOCs tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB84\Desktop\Coursera\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB84\MOOCs-Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6936E0C8-E3CD-4B2F-9BE1-511283AA684C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40397257-1B36-4C2A-AA82-27375AE32472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{81BCB864-2EA9-4732-9E1F-344F7B0A4F91}"/>
   </bookViews>
@@ -752,7 +752,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -789,6 +789,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -802,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -810,6 +816,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1124,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9B4982-F5B0-4EA4-853A-C754B11AA2D5}">
-  <dimension ref="B2:O166"/>
+  <dimension ref="B1:O166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93:G93"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1141,10 +1148,14 @@
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="D1" s="7"/>
+    </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D2" s="7"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">

</xml_diff>

<commit_message>
Updated tracker with Blockchain course
</commit_message>
<xml_diff>
--- a/MOOCs tracker.xlsx
+++ b/MOOCs tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB84\MOOCs-Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB84\Dev-folder\MOOCs-Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40397257-1B36-4C2A-AA82-27375AE32472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C16BE88-E742-4085-9845-C55F5E66C71C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{81BCB864-2EA9-4732-9E1F-344F7B0A4F91}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Coursera" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coursera!$C$5:$M$166</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coursera!$C$5:$M$170</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="234">
   <si>
     <t>Coursera Study Plan</t>
   </si>
@@ -729,6 +729,18 @@
   </si>
   <si>
     <t>Rotterdam</t>
+  </si>
+  <si>
+    <t>Cryptography and Hashing Overvieiw</t>
+  </si>
+  <si>
+    <t>The Blockchain</t>
+  </si>
+  <si>
+    <t>The Merkle Tree and Cryptocurrencies</t>
+  </si>
+  <si>
+    <t>The Blockchain system</t>
   </si>
 </sst>
 </file>
@@ -752,7 +764,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -789,12 +801,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -816,7 +822,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1131,11 +1137,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9B4982-F5B0-4EA4-853A-C754B11AA2D5}">
-  <dimension ref="B1:O166"/>
+  <dimension ref="B1:O170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1595,6 +1599,9 @@
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
       <c r="C25" t="s">
         <v>39</v>
       </c>
@@ -1615,6 +1622,9 @@
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
       <c r="C26" t="s">
         <v>39</v>
       </c>
@@ -1632,6 +1642,9 @@
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
       <c r="C27" t="s">
         <v>39</v>
       </c>
@@ -1649,6 +1662,9 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
       <c r="C28" t="s">
         <v>39</v>
       </c>
@@ -1666,6 +1682,9 @@
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
       <c r="C29" t="s">
         <v>39</v>
       </c>
@@ -1677,6 +1696,9 @@
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
       <c r="C30" t="s">
         <v>39</v>
       </c>
@@ -1688,6 +1710,9 @@
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
       <c r="C31" t="s">
         <v>39</v>
       </c>
@@ -1703,19 +1728,19 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>58</v>
+        <v>231</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
@@ -1723,22 +1748,19 @@
         <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>60</v>
+        <v>230</v>
       </c>
       <c r="F33" t="s">
         <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>59</v>
-      </c>
-      <c r="J33" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.35">
@@ -1746,19 +1768,19 @@
         <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>232</v>
       </c>
       <c r="F34" t="s">
         <v>46</v>
       </c>
       <c r="G34" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.35">
@@ -1766,19 +1788,19 @@
         <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>233</v>
       </c>
       <c r="F35" t="s">
         <v>48</v>
       </c>
       <c r="G35" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.35">
@@ -1788,17 +1810,17 @@
       <c r="C36" t="s">
         <v>56</v>
       </c>
-      <c r="D36" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" t="s">
-        <v>63</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="D36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G36" t="s">
-        <v>17</v>
+      <c r="G36" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.35">
@@ -1809,16 +1831,19 @@
         <v>56</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E37" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F37" t="s">
         <v>44</v>
       </c>
       <c r="G37" t="s">
-        <v>17</v>
+        <v>59</v>
+      </c>
+      <c r="J37" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.35">
@@ -1829,16 +1854,16 @@
         <v>56</v>
       </c>
       <c r="D38" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F38" t="s">
         <v>46</v>
       </c>
       <c r="G38" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
@@ -1849,16 +1874,16 @@
         <v>56</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F39" t="s">
         <v>48</v>
       </c>
       <c r="G39" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
@@ -1866,19 +1891,19 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E40" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="G40" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
@@ -1886,19 +1911,19 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E41" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F41" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="G41" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
@@ -1906,19 +1931,19 @@
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E42" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F42" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G42" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
@@ -1926,19 +1951,19 @@
         <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F43" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="G43" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.35">
@@ -1946,26 +1971,19 @@
         <v>38</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I44" t="s">
-        <v>75</v>
-      </c>
-      <c r="M44" t="s">
-        <v>76</v>
-      </c>
-      <c r="N44" t="s">
-        <v>77</v>
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.35">
@@ -1973,23 +1991,19 @@
         <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="I45" t="s">
-        <v>75</v>
-      </c>
-      <c r="J45" t="s">
-        <v>36</v>
+        <v>65</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>69</v>
+      </c>
+      <c r="F45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.35">
@@ -1997,16 +2011,19 @@
         <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D46" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="F46" t="s">
+        <v>20</v>
       </c>
       <c r="G46" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.35">
@@ -2014,16 +2031,19 @@
         <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D47" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>66</v>
+      </c>
+      <c r="F47" t="s">
+        <v>21</v>
       </c>
       <c r="G47" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.35">
@@ -2033,16 +2053,24 @@
       <c r="C48" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F48" s="3"/>
-      <c r="G48" t="s">
-        <v>82</v>
-      </c>
-      <c r="H48" t="s">
-        <v>83</v>
+      <c r="D48" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I48" t="s">
+        <v>75</v>
+      </c>
+      <c r="M48" t="s">
+        <v>76</v>
+      </c>
+      <c r="N48" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.35">
@@ -2052,14 +2080,21 @@
       <c r="C49" t="s">
         <v>71</v>
       </c>
-      <c r="E49" t="s">
-        <v>84</v>
-      </c>
-      <c r="G49" t="s">
-        <v>82</v>
+      <c r="D49" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I49" t="s">
+        <v>75</v>
       </c>
       <c r="J49" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.35">
@@ -2069,11 +2104,14 @@
       <c r="C50" t="s">
         <v>71</v>
       </c>
+      <c r="D50" t="s">
+        <v>72</v>
+      </c>
       <c r="E50" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G50" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.35">
@@ -2084,13 +2122,13 @@
         <v>71</v>
       </c>
       <c r="D51" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E51" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G51" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.35">
@@ -2100,17 +2138,16 @@
       <c r="C52" t="s">
         <v>71</v>
       </c>
-      <c r="D52" t="s">
-        <v>87</v>
-      </c>
-      <c r="E52" t="s">
-        <v>87</v>
-      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F52" s="3"/>
       <c r="G52" t="s">
-        <v>89</v>
-      </c>
-      <c r="J52" t="s">
-        <v>90</v>
+        <v>82</v>
+      </c>
+      <c r="H52" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.35">
@@ -2120,14 +2157,14 @@
       <c r="C53" t="s">
         <v>71</v>
       </c>
-      <c r="D53" t="s">
-        <v>87</v>
-      </c>
       <c r="E53" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G53" t="s">
-        <v>89</v>
+        <v>82</v>
+      </c>
+      <c r="J53" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.35">
@@ -2137,14 +2174,11 @@
       <c r="C54" t="s">
         <v>71</v>
       </c>
-      <c r="D54" t="s">
-        <v>87</v>
-      </c>
       <c r="E54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G54" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.35">
@@ -2152,19 +2186,16 @@
         <v>38</v>
       </c>
       <c r="C55" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D55" t="s">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="E55" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G55" t="s">
-        <v>53</v>
-      </c>
-      <c r="I55" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.35">
@@ -2172,22 +2203,19 @@
         <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D56" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E56" t="s">
-        <v>94</v>
-      </c>
-      <c r="F56" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="G56" t="s">
-        <v>95</v>
-      </c>
-      <c r="I56" t="s">
-        <v>75</v>
+        <v>89</v>
+      </c>
+      <c r="J56" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.35">
@@ -2195,22 +2223,16 @@
         <v>38</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D57" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E57" t="s">
-        <v>96</v>
-      </c>
-      <c r="F57" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="G57" t="s">
-        <v>95</v>
-      </c>
-      <c r="I57" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.35">
@@ -2218,25 +2240,16 @@
         <v>38</v>
       </c>
       <c r="C58" t="s">
-        <v>92</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I58" t="s">
-        <v>75</v>
-      </c>
-      <c r="N58" t="s">
-        <v>98</v>
+        <v>71</v>
+      </c>
+      <c r="D58" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" t="s">
+        <v>87</v>
+      </c>
+      <c r="G58" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.35">
@@ -2247,16 +2260,13 @@
         <v>92</v>
       </c>
       <c r="D59" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>99</v>
-      </c>
-      <c r="F59" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="G59" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="I59" t="s">
         <v>75</v>
@@ -2276,7 +2286,7 @@
         <v>94</v>
       </c>
       <c r="F60" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G60" t="s">
         <v>95</v>
@@ -2292,25 +2302,21 @@
       <c r="C61" t="s">
         <v>92</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5" t="s">
-        <v>101</v>
+      <c r="D61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" t="s">
+        <v>95</v>
       </c>
       <c r="I61" t="s">
         <v>75</v>
       </c>
-      <c r="J61" t="s">
-        <v>36</v>
-      </c>
-      <c r="K61" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
@@ -2319,23 +2325,23 @@
       <c r="C62" t="s">
         <v>92</v>
       </c>
-      <c r="D62" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" t="s">
-        <v>103</v>
-      </c>
-      <c r="G62" t="s">
-        <v>101</v>
+      <c r="D62" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="I62" t="s">
         <v>75</v>
       </c>
-      <c r="J62" t="s">
-        <v>36</v>
-      </c>
-      <c r="K62" t="s">
-        <v>102</v>
+      <c r="N62" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.35">
@@ -2346,16 +2352,16 @@
         <v>92</v>
       </c>
       <c r="D63" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E63" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F63" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="G63" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I63" t="s">
         <v>75</v>
@@ -2368,24 +2374,21 @@
       <c r="C64" t="s">
         <v>92</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>107</v>
+      <c r="D64" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" t="s">
+        <v>94</v>
+      </c>
+      <c r="F64" t="s">
+        <v>21</v>
+      </c>
+      <c r="G64" t="s">
+        <v>95</v>
       </c>
       <c r="I64" t="s">
         <v>75</v>
       </c>
-      <c r="N64" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
@@ -2394,21 +2397,25 @@
       <c r="C65" t="s">
         <v>92</v>
       </c>
-      <c r="D65" t="s">
-        <v>104</v>
-      </c>
-      <c r="E65" t="s">
-        <v>111</v>
-      </c>
-      <c r="F65" t="s">
-        <v>112</v>
-      </c>
-      <c r="G65" t="s">
-        <v>107</v>
+      <c r="D65" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="I65" t="s">
         <v>75</v>
       </c>
+      <c r="J65" t="s">
+        <v>36</v>
+      </c>
+      <c r="K65" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
@@ -2417,241 +2424,280 @@
       <c r="C66" t="s">
         <v>92</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5" t="s">
-        <v>114</v>
+      <c r="E66" t="s">
+        <v>103</v>
+      </c>
+      <c r="G66" t="s">
+        <v>101</v>
       </c>
       <c r="I66" t="s">
         <v>75</v>
       </c>
+      <c r="J66" t="s">
+        <v>36</v>
+      </c>
+      <c r="K66" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>38</v>
+      </c>
       <c r="C67" t="s">
         <v>92</v>
       </c>
       <c r="D67" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="E67" t="s">
-        <v>115</v>
+        <v>105</v>
+      </c>
+      <c r="F67" t="s">
+        <v>106</v>
       </c>
       <c r="G67" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="I67" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>38</v>
+      </c>
       <c r="C68" t="s">
-        <v>117</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J68" t="s">
-        <v>36</v>
+        <v>92</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I68" t="s">
+        <v>75</v>
       </c>
       <c r="N68" t="s">
-        <v>121</v>
-      </c>
-      <c r="O68" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>38</v>
+      </c>
       <c r="C69" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="D69" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E69" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F69" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="G69" t="s">
-        <v>120</v>
+        <v>107</v>
+      </c>
+      <c r="I69" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
       <c r="C70" t="s">
-        <v>117</v>
-      </c>
-      <c r="D70" t="s">
-        <v>118</v>
-      </c>
-      <c r="E70" t="s">
-        <v>118</v>
-      </c>
-      <c r="F70" t="s">
-        <v>46</v>
-      </c>
-      <c r="G70" t="s">
-        <v>120</v>
+        <v>92</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I70" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C71" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="D71" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="E71" t="s">
-        <v>123</v>
-      </c>
-      <c r="F71" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="G71" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="I71" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C72" t="s">
-        <v>124</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F72" s="2"/>
+        <v>117</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="G72" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J72" t="s">
         <v>36</v>
       </c>
-      <c r="M72" s="2" t="s">
-        <v>127</v>
+      <c r="N72" t="s">
+        <v>121</v>
+      </c>
+      <c r="O72" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C73" t="s">
-        <v>124</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J73" t="s">
-        <v>36</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
+      </c>
+      <c r="D73" t="s">
+        <v>118</v>
+      </c>
+      <c r="E73" t="s">
+        <v>118</v>
+      </c>
+      <c r="F73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G73" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C74" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="D74" t="s">
-        <v>5</v>
+        <v>118</v>
+      </c>
+      <c r="E74" t="s">
+        <v>118</v>
+      </c>
+      <c r="F74" t="s">
+        <v>46</v>
       </c>
       <c r="G74" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C75" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="D75" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="E75" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F75" t="s">
-        <v>135</v>
+        <v>48</v>
       </c>
       <c r="G75" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C76" t="s">
-        <v>137</v>
-      </c>
-      <c r="D76" t="s">
-        <v>138</v>
-      </c>
-      <c r="E76" t="s">
-        <v>138</v>
-      </c>
-      <c r="G76" t="s">
-        <v>139</v>
+        <v>124</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J76" t="s">
+        <v>36</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C77" t="s">
-        <v>137</v>
-      </c>
-      <c r="D77" t="s">
-        <v>138</v>
-      </c>
-      <c r="E77" t="s">
-        <v>138</v>
-      </c>
-      <c r="G77" t="s">
-        <v>139</v>
+        <v>124</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J77" t="s">
+        <v>36</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C78" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D78" t="s">
-        <v>138</v>
-      </c>
-      <c r="E78" t="s">
-        <v>138</v>
+        <v>5</v>
       </c>
       <c r="G78" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C79" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D79" t="s">
-        <v>138</v>
+        <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>138</v>
+        <v>134</v>
+      </c>
+      <c r="F79" t="s">
+        <v>135</v>
       </c>
       <c r="G79" t="s">
-        <v>139</v>
-      </c>
-      <c r="J79" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.35">
@@ -2668,7 +2714,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C81" t="s">
         <v>137</v>
       </c>
@@ -2682,127 +2728,118 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C82" t="s">
+        <v>137</v>
+      </c>
+      <c r="D82" t="s">
+        <v>138</v>
+      </c>
+      <c r="E82" t="s">
+        <v>138</v>
+      </c>
+      <c r="G82" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C83" t="s">
+        <v>137</v>
+      </c>
+      <c r="D83" t="s">
+        <v>138</v>
+      </c>
+      <c r="E83" t="s">
+        <v>138</v>
+      </c>
+      <c r="G83" t="s">
+        <v>139</v>
+      </c>
+      <c r="J83" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C84" t="s">
+        <v>137</v>
+      </c>
+      <c r="D84" t="s">
+        <v>138</v>
+      </c>
+      <c r="E84" t="s">
+        <v>138</v>
+      </c>
+      <c r="G84" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="85" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C85" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" t="s">
+        <v>138</v>
+      </c>
+      <c r="E85" t="s">
+        <v>138</v>
+      </c>
+      <c r="G85" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="86" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C86" t="s">
         <v>124</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E86" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3" t="s">
+      <c r="F86" s="3"/>
+      <c r="G86" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C83" t="s">
+    <row r="87" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C87" t="s">
         <v>124</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D87" t="s">
         <v>5</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E87" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3" t="s">
+      <c r="F87" s="3"/>
+      <c r="G87" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C84" t="s">
+    <row r="88" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C88" t="s">
         <v>144</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E88" t="s">
         <v>145</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G88" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C85" t="s">
+    <row r="89" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C89" t="s">
         <v>124</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D89" t="s">
         <v>5</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E89" t="s">
         <v>147</v>
       </c>
-      <c r="G85" s="6" t="s">
+      <c r="G89" s="6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C86" t="s">
-        <v>149</v>
-      </c>
-      <c r="D86" t="s">
-        <v>150</v>
-      </c>
-      <c r="E86" t="s">
-        <v>151</v>
-      </c>
-      <c r="F86" t="s">
-        <v>16</v>
-      </c>
-      <c r="G86" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C87" t="s">
-        <v>149</v>
-      </c>
-      <c r="D87" t="s">
-        <v>150</v>
-      </c>
-      <c r="E87" t="s">
-        <v>152</v>
-      </c>
-      <c r="F87" t="s">
-        <v>18</v>
-      </c>
-      <c r="G87" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C88" t="s">
-        <v>149</v>
-      </c>
-      <c r="D88" t="s">
-        <v>150</v>
-      </c>
-      <c r="E88" t="s">
-        <v>153</v>
-      </c>
-      <c r="F88" t="s">
-        <v>19</v>
-      </c>
-      <c r="G88" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C89" t="s">
-        <v>149</v>
-      </c>
-      <c r="D89" t="s">
-        <v>150</v>
-      </c>
-      <c r="E89" t="s">
-        <v>150</v>
-      </c>
-      <c r="F89" t="s">
-        <v>20</v>
-      </c>
-      <c r="G89" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C90" t="s">
         <v>149</v>
       </c>
@@ -2810,84 +2847,84 @@
         <v>150</v>
       </c>
       <c r="E90" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F90" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G90" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C91" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D91" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E91" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F91" t="s">
-        <v>155</v>
+        <v>18</v>
       </c>
       <c r="G91" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C92" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D92" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E92" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F92" t="s">
-        <v>157</v>
+        <v>19</v>
       </c>
       <c r="G92" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C93" t="s">
-        <v>14</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G93" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D93" t="s">
+        <v>150</v>
+      </c>
+      <c r="E93" t="s">
+        <v>150</v>
+      </c>
+      <c r="F93" t="s">
+        <v>20</v>
+      </c>
+      <c r="G93" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C94" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="D94" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E94" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F94" t="s">
-        <v>160</v>
+        <v>21</v>
       </c>
       <c r="G94" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C95" t="s">
         <v>14</v>
       </c>
@@ -2898,13 +2935,13 @@
         <v>154</v>
       </c>
       <c r="F95" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G95" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C96" t="s">
         <v>14</v>
       </c>
@@ -2912,212 +2949,212 @@
         <v>154</v>
       </c>
       <c r="E96" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F96" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="G96" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B97" t="s">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C97" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C98" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98" t="s">
+        <v>154</v>
+      </c>
+      <c r="E98" t="s">
+        <v>154</v>
+      </c>
+      <c r="F98" t="s">
+        <v>160</v>
+      </c>
+      <c r="G98" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C99" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" t="s">
+        <v>154</v>
+      </c>
+      <c r="E99" t="s">
+        <v>154</v>
+      </c>
+      <c r="F99" t="s">
+        <v>161</v>
+      </c>
+      <c r="G99" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C100" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" t="s">
+        <v>154</v>
+      </c>
+      <c r="E100" t="s">
+        <v>162</v>
+      </c>
+      <c r="F100" t="s">
+        <v>163</v>
+      </c>
+      <c r="G100" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
         <v>13</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C101" t="s">
         <v>164</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D101" t="s">
         <v>165</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E101" t="s">
         <v>165</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F101" t="s">
         <v>106</v>
-      </c>
-      <c r="G97" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B98" t="s">
-        <v>13</v>
-      </c>
-      <c r="C98" t="s">
-        <v>164</v>
-      </c>
-      <c r="D98" t="s">
-        <v>165</v>
-      </c>
-      <c r="E98" t="s">
-        <v>165</v>
-      </c>
-      <c r="F98" t="s">
-        <v>109</v>
-      </c>
-      <c r="G98" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B99" t="s">
-        <v>13</v>
-      </c>
-      <c r="C99" t="s">
-        <v>164</v>
-      </c>
-      <c r="D99" t="s">
-        <v>165</v>
-      </c>
-      <c r="E99" t="s">
-        <v>165</v>
-      </c>
-      <c r="F99" t="s">
-        <v>112</v>
-      </c>
-      <c r="G99" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C100" t="s">
-        <v>166</v>
-      </c>
-      <c r="D100" t="s">
-        <v>167</v>
-      </c>
-      <c r="E100" t="s">
-        <v>167</v>
-      </c>
-      <c r="F100" t="s">
-        <v>41</v>
-      </c>
-      <c r="G100" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C101" t="s">
-        <v>166</v>
-      </c>
-      <c r="D101" t="s">
-        <v>167</v>
-      </c>
-      <c r="E101" t="s">
-        <v>167</v>
-      </c>
-      <c r="F101" t="s">
-        <v>44</v>
       </c>
       <c r="G101" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B102" t="s">
+        <v>13</v>
+      </c>
       <c r="C102" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D102" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E102" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F102" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="G102" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B103" t="s">
+        <v>13</v>
+      </c>
       <c r="C103" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D103" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E103" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F103" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="G103" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C104" t="s">
         <v>166</v>
       </c>
       <c r="D104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E104" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F104" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="G104" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
         <v>166</v>
       </c>
       <c r="D105" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E105" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F105" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="G105" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
         <v>166</v>
       </c>
       <c r="D106" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E106" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F106" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G106" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
         <v>166</v>
       </c>
       <c r="D107" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E107" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F107" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="G107" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
         <v>166</v>
       </c>
@@ -3125,308 +3162,308 @@
         <v>168</v>
       </c>
       <c r="E108" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F108" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G108" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
-        <v>170</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="N109" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+      <c r="D109" t="s">
+        <v>168</v>
+      </c>
+      <c r="E109" t="s">
+        <v>168</v>
+      </c>
+      <c r="F109" t="s">
+        <v>18</v>
+      </c>
+      <c r="G109" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D110" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E110" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F110" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G110" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C111" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E111" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="F111" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G111" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C112" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D112" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E112" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F112" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G112" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C113" t="s">
         <v>170</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E113" t="s">
-        <v>177</v>
-      </c>
-      <c r="F113" t="s">
-        <v>21</v>
-      </c>
-      <c r="G113" t="s">
+      <c r="E113" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G113" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="N113" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="114" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C114" t="s">
         <v>170</v>
       </c>
       <c r="D114" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E114" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F114" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="G114" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="115" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C115" t="s">
         <v>170</v>
       </c>
       <c r="D115" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E115" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F115" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="G115" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="116" spans="3:7" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="116" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C116" t="s">
         <v>170</v>
       </c>
       <c r="D116" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E116" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F116" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="G116" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="117" spans="3:7" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
         <v>170</v>
       </c>
       <c r="D117" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E117" t="s">
         <v>177</v>
       </c>
       <c r="F117" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G117" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="118" spans="3:7" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="118" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C118" t="s">
         <v>170</v>
       </c>
       <c r="D118" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E118" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F118" t="s">
         <v>41</v>
       </c>
       <c r="G118" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="119" spans="3:7" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="119" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C119" t="s">
         <v>170</v>
       </c>
       <c r="D119" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E119" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F119" t="s">
         <v>44</v>
       </c>
       <c r="G119" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="120" spans="3:7" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="120" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C120" t="s">
         <v>170</v>
       </c>
       <c r="D120" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E120" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F120" t="s">
         <v>46</v>
       </c>
       <c r="G120" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="121" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C121" t="s">
         <v>170</v>
       </c>
       <c r="D121" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E121" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F121" t="s">
         <v>48</v>
       </c>
       <c r="G121" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="122" spans="3:7" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="122" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C122" t="s">
         <v>170</v>
       </c>
       <c r="D122" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E122" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F122" t="s">
-        <v>155</v>
+        <v>41</v>
       </c>
       <c r="G122" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="123" spans="3:7" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="123" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C123" t="s">
         <v>170</v>
       </c>
       <c r="D123" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E123" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F123" t="s">
-        <v>157</v>
+        <v>44</v>
       </c>
       <c r="G123" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="124" spans="3:7" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="124" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C124" t="s">
         <v>170</v>
       </c>
       <c r="D124" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E124" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F124" t="s">
-        <v>159</v>
+        <v>46</v>
       </c>
       <c r="G124" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="125" spans="3:7" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="125" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C125" t="s">
         <v>170</v>
       </c>
       <c r="D125" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E125" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F125" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
       <c r="G125" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="126" spans="3:7" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="126" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C126" t="s">
         <v>170</v>
       </c>
@@ -3434,16 +3471,16 @@
         <v>187</v>
       </c>
       <c r="E126" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F126" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G126" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="127" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C127" t="s">
         <v>170</v>
       </c>
@@ -3451,152 +3488,152 @@
         <v>187</v>
       </c>
       <c r="E127" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F127" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="G127" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="128" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C128" t="s">
         <v>170</v>
       </c>
       <c r="D128" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E128" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F128" t="s">
-        <v>41</v>
+        <v>159</v>
       </c>
       <c r="G128" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="129" spans="3:8" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="129" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C129" t="s">
         <v>170</v>
       </c>
       <c r="D129" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E129" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F129" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
       <c r="G129" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="130" spans="3:8" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="130" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C130" t="s">
         <v>170</v>
       </c>
       <c r="D130" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E130" t="s">
-        <v>199</v>
-      </c>
-      <c r="F130" s="5" t="s">
-        <v>46</v>
+        <v>193</v>
+      </c>
+      <c r="F130" t="s">
+        <v>161</v>
       </c>
       <c r="G130" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="131" spans="3:8" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="131" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C131" t="s">
         <v>170</v>
       </c>
       <c r="D131" t="s">
+        <v>187</v>
+      </c>
+      <c r="E131" t="s">
+        <v>194</v>
+      </c>
+      <c r="F131" t="s">
+        <v>163</v>
+      </c>
+      <c r="G131" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="132" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C132" t="s">
+        <v>170</v>
+      </c>
+      <c r="D132" t="s">
         <v>195</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E132" t="s">
+        <v>196</v>
+      </c>
+      <c r="F132" t="s">
+        <v>41</v>
+      </c>
+      <c r="G132" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="133" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C133" t="s">
+        <v>170</v>
+      </c>
+      <c r="D133" t="s">
+        <v>195</v>
+      </c>
+      <c r="E133" t="s">
+        <v>198</v>
+      </c>
+      <c r="F133" t="s">
+        <v>44</v>
+      </c>
+      <c r="G133" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="134" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C134" t="s">
+        <v>170</v>
+      </c>
+      <c r="D134" t="s">
+        <v>195</v>
+      </c>
+      <c r="E134" t="s">
+        <v>199</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G134" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="135" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C135" t="s">
+        <v>170</v>
+      </c>
+      <c r="D135" t="s">
+        <v>195</v>
+      </c>
+      <c r="E135" t="s">
         <v>177</v>
       </c>
-      <c r="F131" t="s">
+      <c r="F135" t="s">
         <v>48</v>
       </c>
-      <c r="G131" t="s">
+      <c r="G135" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="132" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C132" t="s">
-        <v>200</v>
-      </c>
-      <c r="D132" t="s">
-        <v>201</v>
-      </c>
-      <c r="E132" t="s">
-        <v>201</v>
-      </c>
-      <c r="F132" t="s">
-        <v>16</v>
-      </c>
-      <c r="G132" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="133" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C133" t="s">
-        <v>200</v>
-      </c>
-      <c r="D133" t="s">
-        <v>201</v>
-      </c>
-      <c r="E133" t="s">
-        <v>201</v>
-      </c>
-      <c r="F133" t="s">
-        <v>18</v>
-      </c>
-      <c r="G133" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="134" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C134" t="s">
-        <v>200</v>
-      </c>
-      <c r="D134" t="s">
-        <v>201</v>
-      </c>
-      <c r="E134" t="s">
-        <v>201</v>
-      </c>
-      <c r="F134" t="s">
-        <v>19</v>
-      </c>
-      <c r="G134" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="135" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C135" t="s">
-        <v>200</v>
-      </c>
-      <c r="D135" t="s">
-        <v>201</v>
-      </c>
-      <c r="E135" t="s">
-        <v>201</v>
-      </c>
-      <c r="F135" t="s">
-        <v>20</v>
-      </c>
-      <c r="G135" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="136" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C136" t="s">
         <v>200</v>
       </c>
@@ -3607,240 +3644,240 @@
         <v>201</v>
       </c>
       <c r="F136" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G136" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="137" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C137" t="s">
         <v>200</v>
       </c>
-      <c r="D137" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="F137" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G137" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="138" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="D137" t="s">
+        <v>201</v>
+      </c>
+      <c r="E137" t="s">
+        <v>201</v>
+      </c>
+      <c r="F137" t="s">
+        <v>18</v>
+      </c>
+      <c r="G137" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="138" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C138" t="s">
         <v>200</v>
       </c>
-      <c r="D138" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F138" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G138" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="139" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="D138" t="s">
+        <v>201</v>
+      </c>
+      <c r="E138" t="s">
+        <v>201</v>
+      </c>
+      <c r="F138" t="s">
+        <v>19</v>
+      </c>
+      <c r="G138" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="139" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C139" t="s">
         <v>200</v>
       </c>
       <c r="D139" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E139" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F139" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="G139" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="140" spans="3:8" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="140" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C140" t="s">
         <v>200</v>
       </c>
       <c r="D140" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E140" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F140" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G140" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="141" spans="3:8" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="141" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C141" t="s">
         <v>200</v>
       </c>
-      <c r="D141" t="s">
-        <v>5</v>
-      </c>
-      <c r="E141" t="s">
-        <v>207</v>
-      </c>
-      <c r="G141" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="142" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="D141" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="142" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C142" t="s">
-        <v>209</v>
-      </c>
-      <c r="D142" t="s">
-        <v>210</v>
-      </c>
-      <c r="E142" t="s">
-        <v>210</v>
-      </c>
-      <c r="F142" t="s">
-        <v>41</v>
-      </c>
-      <c r="G142" t="s">
-        <v>202</v>
-      </c>
-      <c r="H142" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="143" spans="3:8" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="143" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C143" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D143" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E143" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F143" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G143" t="s">
-        <v>202</v>
-      </c>
-      <c r="H143" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="144" spans="3:8" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="144" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C144" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D144" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E144" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F144" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G144" t="s">
-        <v>202</v>
-      </c>
-      <c r="H144" t="s">
-        <v>211</v>
+        <v>53</v>
       </c>
     </row>
     <row r="145" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C145" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D145" t="s">
-        <v>210</v>
+        <v>5</v>
       </c>
       <c r="E145" t="s">
-        <v>210</v>
-      </c>
-      <c r="F145" t="s">
-        <v>48</v>
+        <v>207</v>
       </c>
       <c r="G145" t="s">
-        <v>202</v>
-      </c>
-      <c r="H145" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="146" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C146" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="D146" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E146" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F146" t="s">
         <v>41</v>
       </c>
       <c r="G146" t="s">
-        <v>213</v>
+        <v>202</v>
+      </c>
+      <c r="H146" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C147" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="D147" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E147" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F147" t="s">
         <v>44</v>
       </c>
       <c r="G147" t="s">
-        <v>213</v>
+        <v>202</v>
+      </c>
+      <c r="H147" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="148" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C148" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="D148" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E148" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F148" t="s">
         <v>46</v>
       </c>
       <c r="G148" t="s">
-        <v>213</v>
+        <v>202</v>
+      </c>
+      <c r="H148" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C149" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="D149" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E149" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F149" t="s">
         <v>48</v>
       </c>
       <c r="G149" t="s">
-        <v>213</v>
+        <v>202</v>
+      </c>
+      <c r="H149" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="150" spans="3:15" x14ac:dyDescent="0.35">
@@ -3848,16 +3885,16 @@
         <v>170</v>
       </c>
       <c r="D150" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E150" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F150" t="s">
         <v>41</v>
       </c>
       <c r="G150" t="s">
-        <v>116</v>
+        <v>213</v>
       </c>
     </row>
     <row r="151" spans="3:15" x14ac:dyDescent="0.35">
@@ -3865,16 +3902,16 @@
         <v>170</v>
       </c>
       <c r="D151" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E151" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F151" t="s">
         <v>44</v>
       </c>
       <c r="G151" t="s">
-        <v>116</v>
+        <v>213</v>
       </c>
     </row>
     <row r="152" spans="3:15" x14ac:dyDescent="0.35">
@@ -3882,16 +3919,16 @@
         <v>170</v>
       </c>
       <c r="D152" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E152" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F152" t="s">
         <v>46</v>
       </c>
       <c r="G152" t="s">
-        <v>116</v>
+        <v>213</v>
       </c>
     </row>
     <row r="153" spans="3:15" x14ac:dyDescent="0.35">
@@ -3899,209 +3936,277 @@
         <v>170</v>
       </c>
       <c r="D153" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E153" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F153" t="s">
         <v>48</v>
       </c>
       <c r="G153" t="s">
-        <v>116</v>
+        <v>213</v>
       </c>
     </row>
     <row r="154" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C154" t="s">
         <v>170</v>
       </c>
-      <c r="D154" s="4" t="s">
+      <c r="D154" t="s">
+        <v>214</v>
+      </c>
+      <c r="E154" t="s">
+        <v>215</v>
+      </c>
+      <c r="F154" t="s">
+        <v>41</v>
+      </c>
+      <c r="G154" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="155" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C155" t="s">
+        <v>170</v>
+      </c>
+      <c r="D155" t="s">
+        <v>214</v>
+      </c>
+      <c r="E155" t="s">
+        <v>214</v>
+      </c>
+      <c r="F155" t="s">
+        <v>44</v>
+      </c>
+      <c r="G155" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="156" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C156" t="s">
+        <v>170</v>
+      </c>
+      <c r="D156" t="s">
+        <v>214</v>
+      </c>
+      <c r="E156" t="s">
+        <v>214</v>
+      </c>
+      <c r="F156" t="s">
+        <v>46</v>
+      </c>
+      <c r="G156" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="157" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C157" t="s">
+        <v>170</v>
+      </c>
+      <c r="D157" t="s">
+        <v>214</v>
+      </c>
+      <c r="E157" t="s">
+        <v>216</v>
+      </c>
+      <c r="F157" t="s">
+        <v>48</v>
+      </c>
+      <c r="G157" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="158" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C158" t="s">
+        <v>170</v>
+      </c>
+      <c r="D158" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E154" s="4" t="s">
+      <c r="E158" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="F154" s="2"/>
-      <c r="G154" s="2" t="s">
+      <c r="F158" s="2"/>
+      <c r="G158" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="N154" s="2" t="s">
+      <c r="N158" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O154" t="s">
+      <c r="O158" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="155" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="D155" s="4" t="s">
+    <row r="159" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="D159" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="E155" s="4" t="s">
+      <c r="E159" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="F155" s="4" t="s">
+      <c r="F159" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G155" s="4" t="s">
+      <c r="G159" s="4" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="156" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="D156" t="s">
-        <v>220</v>
-      </c>
-      <c r="E156" t="s">
-        <v>220</v>
-      </c>
-      <c r="F156" t="s">
-        <v>18</v>
-      </c>
-      <c r="G156" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="157" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="D157" t="s">
-        <v>220</v>
-      </c>
-      <c r="E157" t="s">
-        <v>220</v>
-      </c>
-      <c r="F157" t="s">
-        <v>19</v>
-      </c>
-      <c r="G157" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="158" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="D158" t="s">
-        <v>220</v>
-      </c>
-      <c r="E158" t="s">
-        <v>220</v>
-      </c>
-      <c r="F158" t="s">
-        <v>20</v>
-      </c>
-      <c r="G158" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="159" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="D159" t="s">
-        <v>220</v>
-      </c>
-      <c r="E159" t="s">
-        <v>220</v>
-      </c>
-      <c r="F159" t="s">
-        <v>21</v>
-      </c>
-      <c r="G159" t="s">
-        <v>218</v>
-      </c>
-      <c r="H159" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="160" spans="3:15" x14ac:dyDescent="0.35">
       <c r="D160" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E160" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F160" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="G160" t="s">
         <v>218</v>
       </c>
-      <c r="H160" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="161" spans="4:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="161" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D161" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E161" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F161" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="G161" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="162" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D162" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E162" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F162" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="G162" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="163" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="163" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D163" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E163" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F163" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G163" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="164" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D164" s="3" t="s">
+      <c r="H163" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="164" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D164" t="s">
+        <v>223</v>
+      </c>
+      <c r="E164" t="s">
+        <v>224</v>
+      </c>
+      <c r="F164" t="s">
+        <v>41</v>
+      </c>
+      <c r="G164" t="s">
+        <v>218</v>
+      </c>
+      <c r="H164" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="165" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D165" t="s">
+        <v>223</v>
+      </c>
+      <c r="E165" t="s">
+        <v>223</v>
+      </c>
+      <c r="F165" t="s">
+        <v>44</v>
+      </c>
+      <c r="G165" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="166" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D166" t="s">
+        <v>223</v>
+      </c>
+      <c r="E166" t="s">
+        <v>223</v>
+      </c>
+      <c r="F166" t="s">
+        <v>46</v>
+      </c>
+      <c r="G166" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="167" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D167" t="s">
+        <v>223</v>
+      </c>
+      <c r="E167" t="s">
+        <v>223</v>
+      </c>
+      <c r="F167" t="s">
+        <v>48</v>
+      </c>
+      <c r="G167" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="168" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D168" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E164" s="3" t="s">
+      <c r="E168" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F164" s="3"/>
-      <c r="G164" s="3" t="s">
+      <c r="F168" s="3"/>
+      <c r="G168" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="165" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D165" s="3" t="s">
+    <row r="169" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D169" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E165" s="3" t="s">
+      <c r="E169" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F165" s="3"/>
-      <c r="G165" s="3" t="s">
+      <c r="F169" s="3"/>
+      <c r="G169" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="166" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D166" s="3" t="s">
+    <row r="170" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D170" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E166" s="3" t="s">
+      <c r="E170" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F166" s="3"/>
-      <c r="G166" s="3" t="s">
+      <c r="F170" s="3"/>
+      <c r="G170" s="3" t="s">
         <v>229</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C5:M166" xr:uid="{2E0B58E9-F860-4CC3-9060-48E8F7B43A92}"/>
+  <autoFilter ref="C5:M170" xr:uid="{2E0B58E9-F860-4CC3-9060-48E8F7B43A92}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>